<commit_message>
full commit after Florida
</commit_message>
<xml_diff>
--- a/Music and Memory/BehaviouralResults/BehaviouralResults-AllParticipants.xlsx
+++ b/Music and Memory/BehaviouralResults/BehaviouralResults-AllParticipants.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-28300" yWindow="1200" windowWidth="23660" windowHeight="16520" tabRatio="592"/>
+    <workbookView xWindow="1080" yWindow="400" windowWidth="27080" windowHeight="14600" tabRatio="592" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Listening Info" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="484">
   <si>
     <t>ID</t>
   </si>
@@ -1486,12 +1486,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-1009]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1637,6 +1638,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1694,7 +1703,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1722,8 +1731,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -1783,15 +1798,6 @@
     <xf numFmtId="15" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="15" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1805,8 +1811,18 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1820,6 +1836,9 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1833,6 +1852,9 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2103,7 +2125,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2113,7 +2135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="O35" sqref="O35"/>
     </sheetView>
@@ -2129,26 +2151,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
-      <c r="R1" s="53" t="s">
+      <c r="R1" s="66" t="s">
         <v>196</v>
       </c>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="54" t="s">
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="66"/>
+      <c r="V1" s="66"/>
+      <c r="W1" s="66"/>
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="67" t="s">
         <v>197</v>
       </c>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
-      <c r="AG1" s="55"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="68"/>
+      <c r="AC1" s="68"/>
+      <c r="AD1" s="68"/>
+      <c r="AE1" s="68"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
     </row>
     <row r="2" spans="1:33" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
@@ -2330,86 +2352,86 @@
       <c r="AF3" s="14"/>
       <c r="AG3" s="14"/>
     </row>
-    <row r="4" spans="1:33" s="63" customFormat="1">
-      <c r="A4" s="63" t="s">
+    <row r="4" spans="1:33" s="60" customFormat="1">
+      <c r="A4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="63">
+      <c r="B4" s="60">
         <v>37.930999999999997</v>
       </c>
-      <c r="C4" s="63">
+      <c r="C4" s="60">
         <v>42.3</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="60">
         <v>80</v>
       </c>
-      <c r="E4" s="63">
+      <c r="E4" s="60">
         <v>100</v>
       </c>
-      <c r="F4" s="63">
+      <c r="F4" s="60">
         <v>100</v>
       </c>
-      <c r="G4" s="63">
+      <c r="G4" s="60">
         <v>100</v>
       </c>
-      <c r="I4" s="63">
+      <c r="I4" s="60">
         <v>100</v>
       </c>
-      <c r="J4" s="63">
+      <c r="J4" s="60">
         <f>9/17</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="K4" s="63">
+      <c r="K4" s="60">
         <f>11/13</f>
         <v>0.84615384615384615</v>
       </c>
-      <c r="L4" s="63">
+      <c r="L4" s="60">
         <v>95.652199999999993</v>
       </c>
-      <c r="M4" s="63">
+      <c r="M4" s="60">
         <v>58</v>
       </c>
-      <c r="N4" s="63">
+      <c r="N4" s="60">
         <f t="shared" ref="N4:N26" si="0">AVERAGE(I4,L4)</f>
         <v>97.826099999999997</v>
       </c>
-      <c r="O4" s="63">
+      <c r="O4" s="60">
         <f t="shared" ref="O4:O15" si="1">AVERAGE(R4:AG4)</f>
         <v>14.375</v>
       </c>
-      <c r="P4" s="60">
+      <c r="P4" s="57">
         <v>20</v>
       </c>
-      <c r="Q4" s="63">
+      <c r="Q4" s="60">
         <f t="shared" ref="Q4:Q26" si="2">O4/P4</f>
         <v>0.71875</v>
       </c>
-      <c r="V4" s="65"/>
-      <c r="W4" s="65"/>
-      <c r="X4" s="65"/>
-      <c r="Y4" s="65"/>
-      <c r="Z4" s="66">
+      <c r="V4" s="62"/>
+      <c r="W4" s="62"/>
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="63">
         <v>16</v>
       </c>
-      <c r="AA4" s="67">
+      <c r="AA4" s="64">
         <v>14</v>
       </c>
-      <c r="AB4" s="67">
+      <c r="AB4" s="64">
         <v>14</v>
       </c>
-      <c r="AC4" s="67">
+      <c r="AC4" s="64">
         <v>14</v>
       </c>
-      <c r="AD4" s="68">
+      <c r="AD4" s="65">
         <v>14</v>
       </c>
-      <c r="AE4" s="68">
+      <c r="AE4" s="65">
         <v>13</v>
       </c>
-      <c r="AF4" s="68">
+      <c r="AF4" s="65">
         <v>15</v>
       </c>
-      <c r="AG4" s="68">
+      <c r="AG4" s="65">
         <v>15</v>
       </c>
     </row>
@@ -3579,82 +3601,82 @@
       <c r="AF18" s="8"/>
       <c r="AG18" s="8"/>
     </row>
-    <row r="19" spans="1:33" s="63" customFormat="1">
-      <c r="A19" s="63" t="s">
+    <row r="19" spans="1:33" s="60" customFormat="1">
+      <c r="A19" s="60" t="s">
         <v>332</v>
       </c>
-      <c r="B19" s="63">
+      <c r="B19" s="60">
         <v>51.7241</v>
       </c>
-      <c r="C19" s="63">
+      <c r="C19" s="60">
         <v>55.5</v>
       </c>
-      <c r="D19" s="63">
+      <c r="D19" s="60">
         <v>30</v>
       </c>
-      <c r="E19" s="63">
+      <c r="E19" s="60">
         <v>70</v>
       </c>
-      <c r="F19" s="63">
+      <c r="F19" s="60">
         <v>70</v>
       </c>
-      <c r="G19" s="63">
+      <c r="G19" s="60">
         <v>70</v>
       </c>
-      <c r="I19" s="63">
+      <c r="I19" s="60">
         <v>58.620699999999999</v>
       </c>
-      <c r="J19" s="63">
+      <c r="J19" s="60">
         <f>9/17</f>
         <v>0.52941176470588236</v>
       </c>
-      <c r="L19" s="63">
+      <c r="L19" s="60">
         <v>78.260900000000007</v>
       </c>
-      <c r="M19" s="63">
+      <c r="M19" s="60">
         <v>111</v>
       </c>
-      <c r="N19" s="63">
+      <c r="N19" s="60">
         <f t="shared" si="0"/>
         <v>68.440799999999996</v>
       </c>
-      <c r="O19" s="63">
+      <c r="O19" s="60">
         <f t="shared" si="3"/>
         <v>3.875</v>
       </c>
-      <c r="P19" s="60">
+      <c r="P19" s="57">
         <v>17</v>
       </c>
-      <c r="Q19" s="63">
+      <c r="Q19" s="60">
         <f t="shared" si="2"/>
         <v>0.22794117647058823</v>
       </c>
-      <c r="V19" s="65"/>
-      <c r="W19" s="65"/>
-      <c r="X19" s="65"/>
-      <c r="Y19" s="65"/>
-      <c r="Z19" s="63">
-        <v>2</v>
-      </c>
-      <c r="AA19" s="63">
+      <c r="V19" s="62"/>
+      <c r="W19" s="62"/>
+      <c r="X19" s="62"/>
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="60">
+        <v>2</v>
+      </c>
+      <c r="AA19" s="60">
         <v>6</v>
       </c>
-      <c r="AB19" s="63">
-        <v>4</v>
-      </c>
-      <c r="AC19" s="63">
-        <v>4</v>
-      </c>
-      <c r="AD19" s="65">
+      <c r="AB19" s="60">
+        <v>4</v>
+      </c>
+      <c r="AC19" s="60">
+        <v>4</v>
+      </c>
+      <c r="AD19" s="62">
         <v>6</v>
       </c>
-      <c r="AE19" s="65">
-        <v>3</v>
-      </c>
-      <c r="AF19" s="65">
-        <v>5</v>
-      </c>
-      <c r="AG19" s="65">
+      <c r="AE19" s="62">
+        <v>3</v>
+      </c>
+      <c r="AF19" s="62">
+        <v>5</v>
+      </c>
+      <c r="AG19" s="62">
         <v>1</v>
       </c>
     </row>
@@ -3816,84 +3838,84 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:33" s="63" customFormat="1">
-      <c r="A22" s="63" t="s">
+    <row r="22" spans="1:33" s="60" customFormat="1">
+      <c r="A22" s="60" t="s">
         <v>336</v>
       </c>
-      <c r="B22" s="63">
+      <c r="B22" s="60">
         <v>27.586200000000002</v>
       </c>
-      <c r="D22" s="63">
+      <c r="D22" s="60">
         <v>60</v>
       </c>
-      <c r="E22" s="63">
+      <c r="E22" s="60">
         <v>50</v>
       </c>
-      <c r="F22" s="63">
+      <c r="F22" s="60">
         <v>80</v>
       </c>
-      <c r="G22" s="63">
+      <c r="G22" s="60">
         <v>70</v>
       </c>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64">
+      <c r="H22" s="61"/>
+      <c r="I22" s="61">
         <v>55.172400000000003</v>
       </c>
-      <c r="J22" s="63">
+      <c r="J22" s="60">
         <f>6/13</f>
         <v>0.46153846153846156</v>
       </c>
-      <c r="K22" s="63">
+      <c r="K22" s="60">
         <f>7/13</f>
         <v>0.53846153846153844</v>
       </c>
-      <c r="L22" s="63">
+      <c r="L22" s="60">
         <v>78.260900000000007</v>
       </c>
-      <c r="M22" s="63">
+      <c r="M22" s="60">
         <v>121</v>
       </c>
-      <c r="N22" s="63">
+      <c r="N22" s="60">
         <f t="shared" si="0"/>
         <v>66.716650000000001</v>
       </c>
-      <c r="O22" s="63">
+      <c r="O22" s="60">
         <f t="shared" si="3"/>
         <v>18.25</v>
       </c>
-      <c r="P22" s="60">
+      <c r="P22" s="57">
         <v>23</v>
       </c>
-      <c r="Q22" s="63">
+      <c r="Q22" s="60">
         <f t="shared" si="2"/>
         <v>0.79347826086956519</v>
       </c>
-      <c r="V22" s="65"/>
-      <c r="W22" s="65"/>
-      <c r="X22" s="65"/>
-      <c r="Y22" s="65"/>
-      <c r="Z22" s="63">
+      <c r="V22" s="62"/>
+      <c r="W22" s="62"/>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="62"/>
+      <c r="Z22" s="60">
         <v>19</v>
       </c>
-      <c r="AA22" s="63">
+      <c r="AA22" s="60">
         <v>20</v>
       </c>
-      <c r="AB22" s="63">
+      <c r="AB22" s="60">
         <v>22</v>
       </c>
-      <c r="AC22" s="63">
+      <c r="AC22" s="60">
         <v>20</v>
       </c>
-      <c r="AD22" s="65">
+      <c r="AD22" s="62">
         <v>15</v>
       </c>
-      <c r="AE22" s="65">
+      <c r="AE22" s="62">
         <v>16</v>
       </c>
-      <c r="AF22" s="65">
+      <c r="AF22" s="62">
         <v>17</v>
       </c>
-      <c r="AG22" s="65">
+      <c r="AG22" s="62">
         <v>17</v>
       </c>
     </row>
@@ -8967,115 +8989,115 @@
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
     </row>
-    <row r="4" spans="1:39" s="59" customFormat="1">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:39" s="56" customFormat="1">
+      <c r="A4" s="53" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="56">
+      <c r="B4" s="53">
         <v>102</v>
       </c>
-      <c r="C4" s="56" t="s">
+      <c r="C4" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="D4" s="56">
+      <c r="D4" s="53">
         <v>39</v>
       </c>
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="53" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="53" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="56" t="s">
+      <c r="G4" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="H4" s="56" t="s">
+      <c r="H4" s="53" t="s">
         <v>151</v>
       </c>
-      <c r="I4" s="56" t="s">
+      <c r="I4" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="J4" s="56" t="s">
+      <c r="J4" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="K4" s="56" t="s">
+      <c r="K4" s="53" t="s">
         <v>128</v>
       </c>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56">
+      <c r="L4" s="53"/>
+      <c r="M4" s="53">
         <v>7</v>
       </c>
-      <c r="N4" s="56">
-        <v>5</v>
-      </c>
-      <c r="O4" s="56" t="s">
+      <c r="N4" s="53">
+        <v>5</v>
+      </c>
+      <c r="O4" s="53" t="s">
         <v>129</v>
       </c>
-      <c r="P4" s="56" t="s">
+      <c r="P4" s="53" t="s">
         <v>153</v>
       </c>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56" t="s">
+      <c r="Q4" s="53"/>
+      <c r="R4" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="S4" s="56" t="s">
+      <c r="S4" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="T4" s="56" t="s">
+      <c r="T4" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="U4" s="56" t="s">
+      <c r="U4" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="V4" s="56" t="s">
+      <c r="V4" s="53" t="s">
         <v>145</v>
       </c>
-      <c r="W4" s="56" t="s">
+      <c r="W4" s="53" t="s">
         <v>146</v>
       </c>
-      <c r="X4" s="56" t="s">
+      <c r="X4" s="53" t="s">
         <v>157</v>
       </c>
-      <c r="Y4" s="56">
-        <v>5</v>
-      </c>
-      <c r="Z4" s="56">
+      <c r="Y4" s="53">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="53">
         <v>6</v>
       </c>
-      <c r="AA4" s="56">
-        <v>5</v>
-      </c>
-      <c r="AB4" s="56">
+      <c r="AA4" s="53">
+        <v>5</v>
+      </c>
+      <c r="AB4" s="53">
         <v>7</v>
       </c>
-      <c r="AC4" s="56">
+      <c r="AC4" s="53">
         <v>6</v>
       </c>
-      <c r="AD4" s="56">
+      <c r="AD4" s="53">
         <v>6</v>
       </c>
-      <c r="AE4" s="56">
-        <v>2</v>
-      </c>
-      <c r="AF4" s="56">
+      <c r="AE4" s="53">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="53">
         <v>7</v>
       </c>
-      <c r="AG4" s="56" t="s">
+      <c r="AG4" s="53" t="s">
         <v>138</v>
       </c>
-      <c r="AH4" s="56"/>
-      <c r="AI4" s="57">
+      <c r="AH4" s="53"/>
+      <c r="AI4" s="54">
         <v>42998</v>
       </c>
-      <c r="AJ4" s="58">
+      <c r="AJ4" s="55">
         <v>43018</v>
       </c>
-      <c r="AK4" s="56">
+      <c r="AK4" s="53">
         <f t="shared" ref="AK4:AK28" si="0">DATEDIF(AI4,AJ4,"d")</f>
         <v>20</v>
       </c>
-      <c r="AL4" s="56"/>
-      <c r="AM4" s="56"/>
+      <c r="AL4" s="53"/>
+      <c r="AM4" s="53"/>
     </row>
     <row r="5" spans="1:39">
       <c r="A5" s="1" t="s">
@@ -10734,115 +10756,115 @@
       <c r="AL19" s="1"/>
       <c r="AM19" s="1"/>
     </row>
-    <row r="20" spans="1:39" s="63" customFormat="1">
-      <c r="A20" s="60" t="s">
+    <row r="20" spans="1:39" s="60" customFormat="1">
+      <c r="A20" s="57" t="s">
         <v>351</v>
       </c>
-      <c r="B20" s="60">
+      <c r="B20" s="57">
         <v>118</v>
       </c>
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="57" t="s">
         <v>352</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="57">
         <v>26</v>
       </c>
-      <c r="E20" s="60" t="s">
+      <c r="E20" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="F20" s="60" t="s">
+      <c r="F20" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="G20" s="60" t="s">
+      <c r="G20" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="H20" s="60" t="s">
+      <c r="H20" s="57" t="s">
         <v>353</v>
       </c>
-      <c r="I20" s="60" t="s">
+      <c r="I20" s="57" t="s">
         <v>354</v>
       </c>
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="K20" s="60" t="s">
+      <c r="K20" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="L20" s="60" t="s">
+      <c r="L20" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="M20" s="60">
+      <c r="M20" s="57">
         <v>7</v>
       </c>
-      <c r="N20" s="60">
-        <v>1</v>
-      </c>
-      <c r="O20" s="60" t="s">
+      <c r="N20" s="57">
+        <v>1</v>
+      </c>
+      <c r="O20" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="60" t="s">
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="S20" s="60" t="s">
+      <c r="S20" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="T20" s="60" t="s">
+      <c r="T20" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="U20" s="60" t="s">
+      <c r="U20" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="V20" s="60" t="s">
+      <c r="V20" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="W20" s="60" t="s">
+      <c r="W20" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="X20" s="60" t="s">
+      <c r="X20" s="57" t="s">
         <v>137</v>
       </c>
-      <c r="Y20" s="60">
+      <c r="Y20" s="57">
         <v>7</v>
       </c>
-      <c r="Z20" s="60">
+      <c r="Z20" s="57">
         <v>6</v>
       </c>
-      <c r="AA20" s="60">
+      <c r="AA20" s="57">
         <v>7</v>
       </c>
-      <c r="AB20" s="60">
-        <v>5</v>
-      </c>
-      <c r="AC20" s="60">
+      <c r="AB20" s="57">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="57">
         <v>7</v>
       </c>
-      <c r="AD20" s="60">
-        <v>5</v>
-      </c>
-      <c r="AE20" s="60">
-        <v>5</v>
-      </c>
-      <c r="AF20" s="60">
-        <v>5</v>
-      </c>
-      <c r="AG20" s="60" t="s">
+      <c r="AD20" s="57">
+        <v>5</v>
+      </c>
+      <c r="AE20" s="57">
+        <v>5</v>
+      </c>
+      <c r="AF20" s="57">
+        <v>5</v>
+      </c>
+      <c r="AG20" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="AH20" s="60"/>
-      <c r="AI20" s="61">
+      <c r="AH20" s="57"/>
+      <c r="AI20" s="58">
         <v>43242</v>
       </c>
-      <c r="AJ20" s="62">
+      <c r="AJ20" s="59">
         <v>43259</v>
       </c>
-      <c r="AK20" s="60">
+      <c r="AK20" s="57">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="AL20" s="60"/>
-      <c r="AM20" s="60"/>
+      <c r="AL20" s="57"/>
+      <c r="AM20" s="57"/>
     </row>
     <row r="21" spans="1:39">
       <c r="A21" s="1" t="s">
@@ -11169,119 +11191,119 @@
       <c r="AL23" s="5"/>
       <c r="AM23" s="5"/>
     </row>
-    <row r="24" spans="1:39" s="63" customFormat="1">
-      <c r="A24" s="60" t="s">
+    <row r="24" spans="1:39" s="60" customFormat="1">
+      <c r="A24" s="57" t="s">
         <v>370</v>
       </c>
-      <c r="B24" s="60">
+      <c r="B24" s="57">
         <v>122</v>
       </c>
-      <c r="C24" s="60" t="s">
+      <c r="C24" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="D24" s="60">
+      <c r="D24" s="57">
         <v>27</v>
       </c>
-      <c r="E24" s="60" t="s">
+      <c r="E24" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="F24" s="60" t="s">
+      <c r="F24" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="60" t="s">
+      <c r="G24" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="H24" s="60" t="s">
+      <c r="H24" s="57" t="s">
         <v>372</v>
       </c>
-      <c r="I24" s="60" t="s">
+      <c r="I24" s="57" t="s">
         <v>373</v>
       </c>
-      <c r="J24" s="60" t="s">
+      <c r="J24" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="K24" s="60" t="s">
+      <c r="K24" s="57" t="s">
         <v>161</v>
       </c>
-      <c r="L24" s="60" t="s">
+      <c r="L24" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="M24" s="60">
+      <c r="M24" s="57">
         <v>6</v>
       </c>
-      <c r="N24" s="60">
-        <v>1</v>
-      </c>
-      <c r="O24" s="60" t="s">
+      <c r="N24" s="57">
+        <v>1</v>
+      </c>
+      <c r="O24" s="57" t="s">
         <v>129</v>
       </c>
-      <c r="P24" s="60" t="s">
+      <c r="P24" s="57" t="s">
         <v>374</v>
       </c>
-      <c r="Q24" s="60" t="s">
+      <c r="Q24" s="57" t="s">
         <v>347</v>
       </c>
-      <c r="R24" s="60" t="s">
+      <c r="R24" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="S24" s="60" t="s">
+      <c r="S24" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="T24" s="60" t="s">
+      <c r="T24" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="U24" s="60" t="s">
+      <c r="U24" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="V24" s="60" t="s">
+      <c r="V24" s="57" t="s">
         <v>297</v>
       </c>
-      <c r="W24" s="60" t="s">
+      <c r="W24" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="X24" s="60" t="s">
+      <c r="X24" s="57" t="s">
         <v>375</v>
       </c>
-      <c r="Y24" s="60">
-        <v>5</v>
-      </c>
-      <c r="Z24" s="60">
-        <v>5</v>
-      </c>
-      <c r="AA24" s="60">
+      <c r="Y24" s="57">
+        <v>5</v>
+      </c>
+      <c r="Z24" s="57">
+        <v>5</v>
+      </c>
+      <c r="AA24" s="57">
         <v>6</v>
       </c>
-      <c r="AB24" s="60">
-        <v>5</v>
-      </c>
-      <c r="AC24" s="60">
-        <v>5</v>
-      </c>
-      <c r="AD24" s="60">
-        <v>5</v>
-      </c>
-      <c r="AE24" s="60">
-        <v>5</v>
-      </c>
-      <c r="AF24" s="60">
-        <v>5</v>
-      </c>
-      <c r="AG24" s="60" t="s">
+      <c r="AB24" s="57">
+        <v>5</v>
+      </c>
+      <c r="AC24" s="57">
+        <v>5</v>
+      </c>
+      <c r="AD24" s="57">
+        <v>5</v>
+      </c>
+      <c r="AE24" s="57">
+        <v>5</v>
+      </c>
+      <c r="AF24" s="57">
+        <v>5</v>
+      </c>
+      <c r="AG24" s="57" t="s">
         <v>138</v>
       </c>
-      <c r="AH24" s="60"/>
-      <c r="AI24" s="61">
+      <c r="AH24" s="57"/>
+      <c r="AI24" s="58">
         <v>43257</v>
       </c>
-      <c r="AJ24" s="62">
+      <c r="AJ24" s="59">
         <v>43280</v>
       </c>
-      <c r="AK24" s="60">
+      <c r="AK24" s="57">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AL24" s="60"/>
-      <c r="AM24" s="60"/>
+      <c r="AL24" s="57"/>
+      <c r="AM24" s="57"/>
     </row>
     <row r="25" spans="1:39">
       <c r="A25" s="1" t="s">
@@ -11810,8 +11832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView topLeftCell="B61" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14245,6 +14267,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -14255,10 +14278,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="K61" sqref="K61"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F5" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14267,81 +14290,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="E1" t="s">
+      <c r="E1" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" s="69" t="s">
+        <v>314</v>
+      </c>
+      <c r="G1" s="69" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="69" t="s">
+        <v>315</v>
+      </c>
+      <c r="I1" s="69" t="s">
+        <v>316</v>
+      </c>
+      <c r="J1" s="69" t="s">
+        <v>314</v>
+      </c>
+      <c r="K1" s="69" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" s="69" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="E2" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>53</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>54</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>55</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>56</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J2" t="s">
         <v>57</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K2" t="s">
         <v>58</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L2" t="s">
         <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2">
-        <v>102</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
-      </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <v>4</v>
-      </c>
-      <c r="J2">
-        <v>3</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3">
         <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E3">
         <v>4</v>
@@ -14350,7 +14361,7 @@
         <v>4</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -14359,7 +14370,7 @@
         <v>4</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>2</v>
@@ -14370,16 +14381,16 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -14408,16 +14419,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B5">
         <v>102</v>
       </c>
       <c r="C5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -14446,92 +14457,92 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B6">
         <v>102</v>
       </c>
       <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>51</v>
       </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>184</v>
-      </c>
-      <c r="B8">
-        <v>104</v>
-      </c>
-      <c r="C8" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>4</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <v>4</v>
-      </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>3</v>
-      </c>
-      <c r="L8">
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9">
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E9">
         <v>3</v>
@@ -14543,7 +14554,7 @@
         <v>3</v>
       </c>
       <c r="H9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <v>4</v>
@@ -14560,28 +14571,28 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10">
         <v>104</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10">
         <v>4</v>
@@ -14590,147 +14601,147 @@
         <v>5</v>
       </c>
       <c r="K10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11">
         <v>104</v>
       </c>
       <c r="C11" t="s">
-        <v>188</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11">
         <v>3</v>
       </c>
       <c r="F11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G11">
         <v>3</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <v>4</v>
       </c>
       <c r="J11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L11">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B12">
         <v>104</v>
       </c>
       <c r="C12" t="s">
+        <v>188</v>
+      </c>
+      <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" t="s">
+        <v>189</v>
+      </c>
+      <c r="B13">
+        <v>104</v>
+      </c>
+      <c r="C13" t="s">
         <v>190</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>67</v>
       </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12">
-        <v>4</v>
-      </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12">
-        <v>3</v>
-      </c>
-      <c r="J12">
-        <v>5</v>
-      </c>
-      <c r="K12">
-        <v>3</v>
-      </c>
-      <c r="L12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14">
-        <v>106</v>
-      </c>
-      <c r="C14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14">
-        <v>5</v>
-      </c>
-      <c r="F14">
-        <v>5</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="H14">
-        <v>4</v>
-      </c>
-      <c r="I14">
-        <v>5</v>
-      </c>
-      <c r="J14">
-        <v>3</v>
-      </c>
-      <c r="K14">
-        <v>2</v>
-      </c>
-      <c r="L14">
-        <v>4</v>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>5</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B15">
         <v>106</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F15">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H15">
         <v>4</v>
@@ -14739,10 +14750,10 @@
         <v>5</v>
       </c>
       <c r="J15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L15">
         <v>4</v>
@@ -14750,16 +14761,16 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B16">
         <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -14771,16 +14782,16 @@
         <v>2</v>
       </c>
       <c r="H16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J16">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L16">
         <v>4</v>
@@ -14788,25 +14799,25 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B17">
         <v>106</v>
       </c>
       <c r="C17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17">
         <v>4</v>
       </c>
       <c r="G17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H17">
         <v>3</v>
@@ -14815,10 +14826,10 @@
         <v>4</v>
       </c>
       <c r="J17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L17">
         <v>4</v>
@@ -14826,101 +14837,95 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18">
         <v>106</v>
       </c>
       <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>106</v>
+      </c>
+      <c r="C19" t="s">
         <v>86</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>67</v>
       </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-      <c r="F18">
-        <v>5</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
-      <c r="K18">
-        <v>3</v>
-      </c>
-      <c r="L18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B20" s="1">
-        <v>108</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="1">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1">
-        <v>4</v>
-      </c>
-      <c r="G20" s="1">
-        <v>3</v>
-      </c>
-      <c r="H20" s="1">
-        <v>2</v>
-      </c>
-      <c r="I20" s="1">
-        <v>4</v>
-      </c>
-      <c r="J20" s="1">
-        <v>4</v>
-      </c>
-      <c r="K20" s="1">
-        <v>3</v>
-      </c>
-      <c r="L20" s="1">
-        <v>1</v>
-      </c>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>3</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B21" s="1">
         <v>108</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F21" s="1">
         <v>4</v>
@@ -14932,7 +14937,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J21" s="1">
         <v>4</v>
@@ -14952,19 +14957,19 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B22" s="1">
         <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E22" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F22" s="1">
         <v>4</v>
@@ -14976,7 +14981,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J22" s="1">
         <v>4</v>
@@ -14996,16 +15001,16 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B23" s="1">
         <v>108</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -15020,7 +15025,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J23" s="1">
         <v>4</v>
@@ -15040,16 +15045,16 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B24" s="1">
         <v>108</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>221</v>
+        <v>241</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -15082,74 +15087,74 @@
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
     </row>
-    <row r="26" spans="1:18">
-      <c r="A26" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="B26" s="1">
-        <v>110</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="1">
-        <v>3</v>
-      </c>
-      <c r="F26" s="1">
-        <v>5</v>
-      </c>
-      <c r="G26" s="1">
-        <v>4</v>
-      </c>
-      <c r="H26" s="1">
-        <v>1</v>
-      </c>
-      <c r="I26" s="1">
-        <v>5</v>
-      </c>
-      <c r="J26" s="1">
-        <v>5</v>
-      </c>
-      <c r="K26" s="1">
-        <v>1</v>
-      </c>
-      <c r="L26" s="1">
-        <v>1</v>
-      </c>
-      <c r="M26" s="1"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
-      <c r="Q26" s="1"/>
-      <c r="R26" s="1"/>
+    <row r="25" spans="1:18">
+      <c r="A25" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B25" s="1">
+        <v>108</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="1">
+        <v>3</v>
+      </c>
+      <c r="F25" s="1">
+        <v>4</v>
+      </c>
+      <c r="G25" s="1">
+        <v>3</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1">
+        <v>3</v>
+      </c>
+      <c r="J25" s="1">
+        <v>4</v>
+      </c>
+      <c r="K25" s="1">
+        <v>3</v>
+      </c>
+      <c r="L25" s="1">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B27" s="1">
         <v>110</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E27" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F27" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G27" s="1">
         <v>4</v>
       </c>
       <c r="H27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27" s="1">
         <v>5</v>
@@ -15158,7 +15163,7 @@
         <v>5</v>
       </c>
       <c r="K27" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L27" s="1">
         <v>1</v>
@@ -15172,22 +15177,22 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B28" s="1">
         <v>110</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E28" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F28" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G28" s="1">
         <v>4</v>
@@ -15202,7 +15207,7 @@
         <v>5</v>
       </c>
       <c r="K28" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L28" s="1">
         <v>1</v>
@@ -15216,16 +15221,16 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B29" s="1">
         <v>110</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>217</v>
+        <v>248</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>213</v>
+        <v>45</v>
       </c>
       <c r="E29" s="1">
         <v>5</v>
@@ -15237,7 +15242,7 @@
         <v>4</v>
       </c>
       <c r="H29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I29" s="1">
         <v>5</v>
@@ -15260,28 +15265,28 @@
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B30" s="1">
         <v>110</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>213</v>
       </c>
       <c r="E30" s="1">
         <v>5</v>
       </c>
       <c r="F30" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G30" s="1">
         <v>4</v>
       </c>
       <c r="H30" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I30" s="1">
         <v>5</v>
@@ -15290,7 +15295,7 @@
         <v>5</v>
       </c>
       <c r="K30" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L30" s="1">
         <v>1</v>
@@ -15302,74 +15307,74 @@
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
     </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B32" s="1">
-        <v>112</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E32" s="1">
-        <v>5</v>
-      </c>
-      <c r="F32" s="1">
-        <v>5</v>
-      </c>
-      <c r="G32" s="1">
-        <v>3</v>
-      </c>
-      <c r="H32" s="1">
-        <v>2</v>
-      </c>
-      <c r="I32" s="1">
-        <v>5</v>
-      </c>
-      <c r="J32" s="1">
-        <v>5</v>
-      </c>
-      <c r="K32" s="1">
-        <v>4</v>
-      </c>
-      <c r="L32" s="1">
-        <v>3</v>
-      </c>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
+    <row r="31" spans="1:18">
+      <c r="A31" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B31" s="1">
+        <v>110</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="1">
+        <v>5</v>
+      </c>
+      <c r="F31" s="1">
+        <v>4</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>5</v>
+      </c>
+      <c r="J31" s="1">
+        <v>5</v>
+      </c>
+      <c r="K31" s="1">
+        <v>3</v>
+      </c>
+      <c r="L31" s="1">
+        <v>1</v>
+      </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B33" s="1">
         <v>112</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>254</v>
+        <v>39</v>
       </c>
       <c r="E33" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F33" s="1">
         <v>5</v>
       </c>
       <c r="G33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H33" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I33" s="1">
         <v>5</v>
@@ -15392,19 +15397,19 @@
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B34" s="1">
         <v>112</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>45</v>
+        <v>254</v>
       </c>
       <c r="E34" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34" s="1">
         <v>5</v>
@@ -15413,7 +15418,7 @@
         <v>4</v>
       </c>
       <c r="H34" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I34" s="1">
         <v>5</v>
@@ -15425,7 +15430,7 @@
         <v>4</v>
       </c>
       <c r="L34" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M34" s="1"/>
       <c r="N34" s="1"/>
@@ -15436,16 +15441,16 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B35" s="1">
         <v>112</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>219</v>
+        <v>248</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E35" s="1">
         <v>5</v>
@@ -15457,7 +15462,7 @@
         <v>4</v>
       </c>
       <c r="H35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I35" s="1">
         <v>5</v>
@@ -15466,10 +15471,10 @@
         <v>5</v>
       </c>
       <c r="K35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L35" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -15480,19 +15485,19 @@
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B36" s="1">
         <v>112</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E36" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F36" s="1">
         <v>5</v>
@@ -15510,7 +15515,7 @@
         <v>5</v>
       </c>
       <c r="K36" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L36" s="1">
         <v>3</v>
@@ -15522,62 +15527,62 @@
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
     </row>
-    <row r="38" spans="1:18">
-      <c r="A38" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="B38" s="1">
-        <v>114</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1</v>
-      </c>
-      <c r="H38" s="1">
-        <v>1</v>
-      </c>
-      <c r="I38" s="1">
-        <v>1</v>
-      </c>
-      <c r="J38" s="1">
-        <v>1</v>
-      </c>
-      <c r="K38" s="1">
-        <v>1</v>
-      </c>
-      <c r="L38" s="1">
-        <v>1</v>
-      </c>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-      <c r="O38" s="1"/>
-      <c r="P38" s="1"/>
-      <c r="Q38" s="1"/>
-      <c r="R38" s="1"/>
+    <row r="37" spans="1:18">
+      <c r="A37" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B37" s="1">
+        <v>112</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="1">
+        <v>4</v>
+      </c>
+      <c r="F37" s="1">
+        <v>5</v>
+      </c>
+      <c r="G37" s="1">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1">
+        <v>3</v>
+      </c>
+      <c r="I37" s="1">
+        <v>5</v>
+      </c>
+      <c r="J37" s="1">
+        <v>5</v>
+      </c>
+      <c r="K37" s="1">
+        <v>4</v>
+      </c>
+      <c r="L37" s="1">
+        <v>3</v>
+      </c>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B39" s="1">
         <v>114</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
@@ -15592,10 +15597,10 @@
         <v>1</v>
       </c>
       <c r="I39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K39" s="1">
         <v>1</v>
@@ -15612,16 +15617,16 @@
     </row>
     <row r="40" spans="1:18">
       <c r="A40" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B40" s="1">
         <v>114</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D40" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E40" s="1">
         <v>1</v>
@@ -15656,16 +15661,16 @@
     </row>
     <row r="41" spans="1:18">
       <c r="A41" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B41" s="1">
         <v>114</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>48</v>
+        <v>210</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -15700,22 +15705,22 @@
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B42" s="1">
         <v>114</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
       </c>
       <c r="F42" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42" s="1">
         <v>1</v>
@@ -15724,10 +15729,10 @@
         <v>1</v>
       </c>
       <c r="I42" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J42" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K42" s="1">
         <v>1</v>
@@ -15742,68 +15747,68 @@
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
     </row>
-    <row r="44" spans="1:18">
-      <c r="A44" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="B44" s="1">
-        <v>116</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E44" s="1">
-        <v>5</v>
-      </c>
-      <c r="F44" s="1">
-        <v>4</v>
-      </c>
-      <c r="G44" s="1">
-        <v>2</v>
-      </c>
-      <c r="H44" s="1">
-        <v>1</v>
-      </c>
-      <c r="I44" s="1">
-        <v>3</v>
-      </c>
-      <c r="J44" s="1">
-        <v>3</v>
-      </c>
-      <c r="K44" s="1">
-        <v>1</v>
-      </c>
-      <c r="L44" s="1">
-        <v>1</v>
-      </c>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
+    <row r="43" spans="1:18">
+      <c r="A43" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B43" s="1">
+        <v>114</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>1</v>
+      </c>
+      <c r="I43" s="1">
+        <v>3</v>
+      </c>
+      <c r="J43" s="1">
+        <v>3</v>
+      </c>
+      <c r="K43" s="1">
+        <v>1</v>
+      </c>
+      <c r="L43" s="1">
+        <v>1</v>
+      </c>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
     </row>
     <row r="45" spans="1:18">
       <c r="A45" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B45" s="1">
         <v>116</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>254</v>
+        <v>61</v>
       </c>
       <c r="E45" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F45" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G45" s="1">
         <v>2</v>
@@ -15812,13 +15817,13 @@
         <v>1</v>
       </c>
       <c r="I45" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J45" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K45" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L45" s="1">
         <v>1</v>
@@ -15832,19 +15837,19 @@
     </row>
     <row r="46" spans="1:18">
       <c r="A46" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B46" s="1">
         <v>116</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>352</v>
+        <v>431</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>433</v>
+        <v>254</v>
       </c>
       <c r="E46" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F46" s="1">
         <v>5</v>
@@ -15876,16 +15881,16 @@
     </row>
     <row r="47" spans="1:18">
       <c r="A47" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B47" s="1">
         <v>116</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="D47" s="1">
-        <v>4</v>
+        <v>352</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>433</v>
       </c>
       <c r="E47" s="1">
         <v>4</v>
@@ -15900,7 +15905,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J47" s="1">
         <v>2</v>
@@ -15920,16 +15925,16 @@
     </row>
     <row r="48" spans="1:18">
       <c r="A48" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B48" s="1">
         <v>116</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>67</v>
+        <v>435</v>
+      </c>
+      <c r="D48" s="1">
+        <v>4</v>
       </c>
       <c r="E48" s="1">
         <v>4</v>
@@ -15962,83 +15967,83 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
     </row>
-    <row r="50" spans="1:18">
-      <c r="A50" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="B50" s="1">
-        <v>118</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="D50" s="1">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1">
-        <v>3</v>
-      </c>
-      <c r="F50" s="1">
-        <v>4</v>
-      </c>
-      <c r="G50" s="1">
-        <v>1</v>
-      </c>
-      <c r="H50" s="1">
-        <v>1</v>
-      </c>
-      <c r="I50" s="1">
-        <v>2</v>
-      </c>
-      <c r="J50" s="1">
-        <v>1</v>
-      </c>
-      <c r="K50" s="1">
-        <v>1</v>
-      </c>
-      <c r="L50" s="1">
-        <v>1</v>
-      </c>
-      <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
-      <c r="Q50" s="1"/>
-      <c r="R50" s="1"/>
+    <row r="49" spans="1:18">
+      <c r="A49" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B49" s="1">
+        <v>116</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E49" s="1">
+        <v>4</v>
+      </c>
+      <c r="F49" s="1">
+        <v>5</v>
+      </c>
+      <c r="G49" s="1">
+        <v>2</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1</v>
+      </c>
+      <c r="I49" s="1">
+        <v>3</v>
+      </c>
+      <c r="J49" s="1">
+        <v>2</v>
+      </c>
+      <c r="K49" s="1">
+        <v>2</v>
+      </c>
+      <c r="L49" s="1">
+        <v>1</v>
+      </c>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1"/>
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B51" s="1">
         <v>118</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>397</v>
+        <v>438</v>
       </c>
       <c r="D51" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E51" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F51" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G51" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H51" s="1">
         <v>1</v>
       </c>
       <c r="I51" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J51" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K51" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L51" s="1">
         <v>1</v>
@@ -16052,25 +16057,25 @@
     </row>
     <row r="52" spans="1:18">
       <c r="A52" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B52" s="1">
         <v>118</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>441</v>
+        <v>397</v>
       </c>
       <c r="D52" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E52" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F52" s="1">
         <v>5</v>
       </c>
       <c r="G52" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H52" s="1">
         <v>1</v>
@@ -16096,25 +16101,25 @@
     </row>
     <row r="53" spans="1:18">
       <c r="A53" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B53" s="1">
         <v>118</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>48</v>
+        <v>441</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3</v>
       </c>
       <c r="E53" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F53" s="1">
         <v>5</v>
       </c>
       <c r="G53" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H53" s="1">
         <v>1</v>
@@ -16123,7 +16128,7 @@
         <v>3</v>
       </c>
       <c r="J53" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K53" s="1">
         <v>3</v>
@@ -16140,19 +16145,19 @@
     </row>
     <row r="54" spans="1:18">
       <c r="A54" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B54" s="1">
         <v>118</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>444</v>
+        <v>401</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="E54" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F54" s="1">
         <v>5</v>
@@ -16182,86 +16187,86 @@
       <c r="Q54" s="1"/>
       <c r="R54" s="1"/>
     </row>
-    <row r="56" spans="1:18">
-      <c r="A56" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="B56" s="1">
-        <v>120</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D56" s="1">
-        <v>1</v>
-      </c>
-      <c r="E56" s="1">
-        <v>3</v>
-      </c>
-      <c r="F56" s="1">
-        <v>4</v>
-      </c>
-      <c r="G56" s="1">
-        <v>4</v>
-      </c>
-      <c r="H56" s="1">
-        <v>3</v>
-      </c>
-      <c r="I56" s="1">
-        <v>3</v>
-      </c>
-      <c r="J56" s="1">
-        <v>3</v>
-      </c>
-      <c r="K56" s="1">
-        <v>3</v>
-      </c>
-      <c r="L56" s="1">
-        <v>3</v>
-      </c>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-      <c r="O56" s="1"/>
-      <c r="P56" s="1"/>
-      <c r="Q56" s="1"/>
-      <c r="R56" s="1"/>
+    <row r="55" spans="1:18">
+      <c r="A55" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="B55" s="1">
+        <v>118</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2</v>
+      </c>
+      <c r="F55" s="1">
+        <v>5</v>
+      </c>
+      <c r="G55" s="1">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+      <c r="I55" s="1">
+        <v>3</v>
+      </c>
+      <c r="J55" s="1">
+        <v>4</v>
+      </c>
+      <c r="K55" s="1">
+        <v>3</v>
+      </c>
+      <c r="L55" s="1">
+        <v>1</v>
+      </c>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1"/>
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B57" s="1">
         <v>120</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D57" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E57" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F57" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G57" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H57" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I57" s="1">
         <v>3</v>
       </c>
       <c r="J57" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K57" s="1">
         <v>3</v>
       </c>
       <c r="L57" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
@@ -16272,25 +16277,25 @@
     </row>
     <row r="58" spans="1:18">
       <c r="A58" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B58" s="1">
         <v>120</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D58" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E58" s="1">
         <v>2</v>
       </c>
       <c r="F58" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G58" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H58" s="1">
         <v>2</v>
@@ -16316,25 +16321,25 @@
     </row>
     <row r="59" spans="1:18">
       <c r="A59" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B59" s="1">
         <v>120</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>213</v>
+        <v>410</v>
+      </c>
+      <c r="D59" s="1">
+        <v>3</v>
       </c>
       <c r="E59" s="1">
         <v>2</v>
       </c>
       <c r="F59" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G59" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H59" s="1">
         <v>2</v>
@@ -16360,16 +16365,16 @@
     </row>
     <row r="60" spans="1:18">
       <c r="A60" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B60" s="1">
         <v>120</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>380</v>
+        <v>449</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>67</v>
+        <v>213</v>
       </c>
       <c r="E60" s="1">
         <v>2</v>
@@ -16384,7 +16389,7 @@
         <v>2</v>
       </c>
       <c r="I60" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J60" s="1">
         <v>2</v>
@@ -16402,68 +16407,68 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
     </row>
-    <row r="62" spans="1:18">
-      <c r="A62" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="B62" s="1">
-        <v>122</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D62" s="1">
-        <v>1</v>
-      </c>
-      <c r="E62" s="1">
-        <v>3</v>
-      </c>
-      <c r="F62" s="1">
-        <v>3</v>
-      </c>
-      <c r="G62" s="1">
-        <v>2</v>
-      </c>
-      <c r="H62" s="1">
-        <v>2</v>
-      </c>
-      <c r="I62" s="1">
-        <v>2</v>
-      </c>
-      <c r="J62" s="1">
-        <v>2</v>
-      </c>
-      <c r="K62" s="1">
-        <v>1</v>
-      </c>
-      <c r="L62" s="1">
-        <v>1</v>
-      </c>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-      <c r="O62" s="1"/>
-      <c r="P62" s="1"/>
-      <c r="Q62" s="1"/>
-      <c r="R62" s="1"/>
+    <row r="61" spans="1:18">
+      <c r="A61" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B61" s="1">
+        <v>120</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E61" s="1">
+        <v>2</v>
+      </c>
+      <c r="F61" s="1">
+        <v>3</v>
+      </c>
+      <c r="G61" s="1">
+        <v>3</v>
+      </c>
+      <c r="H61" s="1">
+        <v>2</v>
+      </c>
+      <c r="I61" s="1">
+        <v>4</v>
+      </c>
+      <c r="J61" s="1">
+        <v>2</v>
+      </c>
+      <c r="K61" s="1">
+        <v>3</v>
+      </c>
+      <c r="L61" s="1">
+        <v>2</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B63" s="1">
         <v>122</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>404</v>
+        <v>362</v>
       </c>
       <c r="D63" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E63" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F63" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G63" s="1">
         <v>2</v>
@@ -16475,13 +16480,13 @@
         <v>2</v>
       </c>
       <c r="J63" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K63" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L63" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M63" s="1"/>
       <c r="N63" s="1"/>
@@ -16492,22 +16497,22 @@
     </row>
     <row r="64" spans="1:18">
       <c r="A64" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B64" s="1">
         <v>122</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="D64" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E64" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F64" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G64" s="1">
         <v>2</v>
@@ -16519,7 +16524,7 @@
         <v>2</v>
       </c>
       <c r="J64" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K64" s="1">
         <v>3</v>
@@ -16536,16 +16541,16 @@
     </row>
     <row r="65" spans="1:18">
       <c r="A65" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B65" s="1">
         <v>122</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>213</v>
+        <v>408</v>
+      </c>
+      <c r="D65" s="1">
+        <v>3</v>
       </c>
       <c r="E65" s="1">
         <v>3</v>
@@ -16554,10 +16559,10 @@
         <v>3</v>
       </c>
       <c r="G65" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H65" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I65" s="1">
         <v>2</v>
@@ -16566,7 +16571,7 @@
         <v>2</v>
       </c>
       <c r="K65" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L65" s="1">
         <v>2</v>
@@ -16580,16 +16585,16 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B66" s="1">
         <v>122</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>380</v>
+        <v>449</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>67</v>
+        <v>213</v>
       </c>
       <c r="E66" s="1">
         <v>3</v>
@@ -16598,16 +16603,16 @@
         <v>3</v>
       </c>
       <c r="G66" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H66" s="1">
         <v>1</v>
       </c>
       <c r="I66" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J66" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K66" s="1">
         <v>2</v>
@@ -16622,65 +16627,65 @@
       <c r="Q66" s="1"/>
       <c r="R66" s="1"/>
     </row>
-    <row r="68" spans="1:18">
-      <c r="A68" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="B68" s="1">
-        <v>124</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D68" s="1">
-        <v>1</v>
-      </c>
-      <c r="E68" s="1">
-        <v>3</v>
-      </c>
-      <c r="F68" s="1">
-        <v>4</v>
-      </c>
-      <c r="G68" s="1">
-        <v>4</v>
-      </c>
-      <c r="H68" s="1">
-        <v>4</v>
-      </c>
-      <c r="I68" s="1">
-        <v>3</v>
-      </c>
-      <c r="J68" s="1">
-        <v>3</v>
-      </c>
-      <c r="K68" s="1">
-        <v>4</v>
-      </c>
-      <c r="L68" s="1">
-        <v>2</v>
-      </c>
-      <c r="M68" s="1"/>
-      <c r="N68" s="1"/>
-      <c r="O68" s="1"/>
-      <c r="P68" s="1"/>
-      <c r="Q68" s="1"/>
-      <c r="R68" s="1"/>
+    <row r="67" spans="1:18">
+      <c r="A67" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="B67" s="1">
+        <v>122</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="1">
+        <v>3</v>
+      </c>
+      <c r="F67" s="1">
+        <v>3</v>
+      </c>
+      <c r="G67" s="1">
+        <v>2</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+      <c r="I67" s="1">
+        <v>3</v>
+      </c>
+      <c r="J67" s="1">
+        <v>3</v>
+      </c>
+      <c r="K67" s="1">
+        <v>2</v>
+      </c>
+      <c r="L67" s="1">
+        <v>2</v>
+      </c>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B69" s="1">
         <v>124</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>412</v>
+        <v>425</v>
       </c>
       <c r="D69" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E69" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F69" s="1">
         <v>4</v>
@@ -16689,7 +16694,7 @@
         <v>4</v>
       </c>
       <c r="H69" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I69" s="1">
         <v>3</v>
@@ -16698,10 +16703,10 @@
         <v>3</v>
       </c>
       <c r="K69" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L69" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M69" s="1"/>
       <c r="N69" s="1"/>
@@ -16712,16 +16717,16 @@
     </row>
     <row r="70" spans="1:18">
       <c r="A70" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B70" s="1">
         <v>124</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="D70" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E70" s="1">
         <v>4</v>
@@ -16730,13 +16735,13 @@
         <v>4</v>
       </c>
       <c r="G70" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H70" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I70" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J70" s="1">
         <v>3</v>
@@ -16745,7 +16750,7 @@
         <v>3</v>
       </c>
       <c r="L70" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M70" s="1"/>
       <c r="N70" s="1"/>
@@ -16756,16 +16761,16 @@
     </row>
     <row r="71" spans="1:18">
       <c r="A71" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B71" s="1">
         <v>124</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>416</v>
+        <v>459</v>
       </c>
       <c r="D71" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E71" s="1">
         <v>4</v>
@@ -16774,7 +16779,7 @@
         <v>4</v>
       </c>
       <c r="G71" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H71" s="1">
         <v>4</v>
@@ -16800,19 +16805,19 @@
     </row>
     <row r="72" spans="1:18">
       <c r="A72" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B72" s="1">
         <v>124</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>67</v>
+        <v>416</v>
+      </c>
+      <c r="D72" s="1">
+        <v>4</v>
       </c>
       <c r="E72" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F72" s="1">
         <v>4</v>
@@ -16827,10 +16832,10 @@
         <v>4</v>
       </c>
       <c r="J72" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K72" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L72" s="1">
         <v>1</v>
@@ -16842,71 +16847,71 @@
       <c r="Q72" s="1"/>
       <c r="R72" s="1"/>
     </row>
-    <row r="74" spans="1:18">
-      <c r="A74" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="B74" s="1">
-        <v>126</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D74" s="1">
-        <v>1</v>
-      </c>
-      <c r="E74" s="1">
-        <v>4</v>
-      </c>
-      <c r="F74" s="1">
-        <v>3</v>
-      </c>
-      <c r="G74" s="1">
-        <v>2</v>
-      </c>
-      <c r="H74" s="1">
-        <v>1</v>
-      </c>
-      <c r="I74" s="1">
-        <v>3</v>
-      </c>
-      <c r="J74" s="1">
-        <v>3</v>
-      </c>
-      <c r="K74" s="1">
-        <v>4</v>
-      </c>
-      <c r="L74" s="1">
-        <v>1</v>
-      </c>
-      <c r="M74" s="1"/>
-      <c r="N74" s="1"/>
-      <c r="O74" s="1"/>
-      <c r="P74" s="1"/>
-      <c r="Q74" s="1"/>
-      <c r="R74" s="1"/>
+    <row r="73" spans="1:18">
+      <c r="A73" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B73" s="1">
+        <v>124</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E73" s="1">
+        <v>5</v>
+      </c>
+      <c r="F73" s="1">
+        <v>4</v>
+      </c>
+      <c r="G73" s="1">
+        <v>4</v>
+      </c>
+      <c r="H73" s="1">
+        <v>4</v>
+      </c>
+      <c r="I73" s="1">
+        <v>4</v>
+      </c>
+      <c r="J73" s="1">
+        <v>2</v>
+      </c>
+      <c r="K73" s="1">
+        <v>2</v>
+      </c>
+      <c r="L73" s="1">
+        <v>1</v>
+      </c>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B75" s="1">
         <v>126</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>459</v>
+        <v>427</v>
       </c>
       <c r="D75" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F75" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G75" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H75" s="1">
         <v>1</v>
@@ -16915,10 +16920,10 @@
         <v>3</v>
       </c>
       <c r="J75" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K75" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L75" s="1">
         <v>1</v>
@@ -16932,16 +16937,16 @@
     </row>
     <row r="76" spans="1:18">
       <c r="A76" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B76" s="1">
         <v>126</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="D76" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E76" s="1">
         <v>3</v>
@@ -16950,16 +16955,16 @@
         <v>4</v>
       </c>
       <c r="G76" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H76" s="1">
         <v>1</v>
       </c>
       <c r="I76" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J76" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K76" s="1">
         <v>3</v>
@@ -16974,39 +16979,39 @@
       <c r="Q76" s="1"/>
       <c r="R76" s="1"/>
     </row>
-    <row r="77" spans="1:18" ht="16" thickBot="1">
+    <row r="77" spans="1:18">
       <c r="A77" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B77" s="1">
         <v>126</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>213</v>
+        <v>466</v>
+      </c>
+      <c r="D77" s="1">
+        <v>3</v>
       </c>
       <c r="E77" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F77" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G77" s="1">
         <v>4</v>
       </c>
       <c r="H77" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I77" s="1">
         <v>4</v>
       </c>
       <c r="J77" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K77" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L77" s="1">
         <v>1</v>
@@ -17019,106 +17024,150 @@
       <c r="R77" s="1"/>
     </row>
     <row r="78" spans="1:18" ht="16" thickBot="1">
-      <c r="A78" s="22">
+      <c r="A78" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B78" s="1">
+        <v>126</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E78" s="1">
+        <v>4</v>
+      </c>
+      <c r="F78" s="1">
+        <v>5</v>
+      </c>
+      <c r="G78" s="1">
+        <v>4</v>
+      </c>
+      <c r="H78" s="1">
+        <v>2</v>
+      </c>
+      <c r="I78" s="1">
+        <v>4</v>
+      </c>
+      <c r="J78" s="1">
+        <v>5</v>
+      </c>
+      <c r="K78" s="1">
+        <v>4</v>
+      </c>
+      <c r="L78" s="1">
+        <v>1</v>
+      </c>
+      <c r="M78" s="1"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="1"/>
+    </row>
+    <row r="79" spans="1:18" ht="16" thickBot="1">
+      <c r="A79" s="22">
         <v>43314.561597222222</v>
       </c>
-      <c r="B78" s="19">
+      <c r="B79" s="19">
         <v>126</v>
       </c>
-      <c r="C78" s="20">
+      <c r="C79" s="20">
         <v>43314</v>
       </c>
-      <c r="D78" s="21" t="s">
+      <c r="D79" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E78" s="19">
-        <v>5</v>
-      </c>
-      <c r="F78" s="19">
-        <v>5</v>
-      </c>
-      <c r="G78" s="19">
-        <v>4</v>
-      </c>
-      <c r="H78" s="19">
-        <v>2</v>
-      </c>
-      <c r="I78" s="19">
-        <v>4</v>
-      </c>
-      <c r="J78" s="19">
-        <v>5</v>
-      </c>
-      <c r="K78" s="19">
-        <v>4</v>
-      </c>
-      <c r="L78" s="19">
-        <v>2</v>
-      </c>
-      <c r="M78" s="21"/>
-      <c r="N78" s="21"/>
-      <c r="O78" s="21"/>
-      <c r="P78" s="21"/>
-      <c r="Q78" s="21"/>
-      <c r="R78" s="21"/>
-    </row>
-    <row r="80" spans="1:18">
-      <c r="E80">
-        <f>AVERAGE(E2:E78)</f>
+      <c r="E79" s="19">
+        <v>5</v>
+      </c>
+      <c r="F79" s="19">
+        <v>5</v>
+      </c>
+      <c r="G79" s="19">
+        <v>4</v>
+      </c>
+      <c r="H79" s="19">
+        <v>2</v>
+      </c>
+      <c r="I79" s="19">
+        <v>4</v>
+      </c>
+      <c r="J79" s="19">
+        <v>5</v>
+      </c>
+      <c r="K79" s="19">
+        <v>4</v>
+      </c>
+      <c r="L79" s="19">
+        <v>2</v>
+      </c>
+      <c r="M79" s="21"/>
+      <c r="N79" s="21"/>
+      <c r="O79" s="21"/>
+      <c r="P79" s="21"/>
+      <c r="Q79" s="21"/>
+      <c r="R79" s="21"/>
+    </row>
+    <row r="81" spans="5:12">
+      <c r="E81">
+        <f>AVERAGE(E3:E79)</f>
         <v>3.3076923076923075</v>
       </c>
-      <c r="F80">
-        <f t="shared" ref="F80:L80" si="0">AVERAGE(F2:F78)</f>
+      <c r="F81">
+        <f t="shared" ref="F81:L81" si="0">AVERAGE(F3:F79)</f>
         <v>3.9846153846153847</v>
       </c>
-      <c r="G80">
+      <c r="G81">
         <f t="shared" si="0"/>
         <v>2.8</v>
       </c>
-      <c r="H80">
+      <c r="H81">
         <f t="shared" si="0"/>
         <v>2.0769230769230771</v>
       </c>
-      <c r="I80">
+      <c r="I81">
         <f t="shared" si="0"/>
         <v>3.523076923076923</v>
       </c>
-      <c r="J80">
+      <c r="J81">
         <f t="shared" si="0"/>
         <v>3.5076923076923077</v>
       </c>
-      <c r="K80">
+      <c r="K81">
         <f t="shared" si="0"/>
         <v>2.6923076923076925</v>
       </c>
-      <c r="L80">
+      <c r="L81">
         <f t="shared" si="0"/>
         <v>1.7692307692307692</v>
       </c>
     </row>
-    <row r="81" spans="5:12">
-      <c r="E81" t="s">
+    <row r="82" spans="5:12">
+      <c r="E82" t="s">
         <v>316</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F82" t="s">
         <v>314</v>
       </c>
-      <c r="G81" t="s">
+      <c r="G82" t="s">
         <v>313</v>
       </c>
-      <c r="H81" t="s">
+      <c r="H82" t="s">
         <v>315</v>
       </c>
-      <c r="I81" t="s">
+      <c r="I82" t="s">
         <v>316</v>
       </c>
-      <c r="J81" t="s">
+      <c r="J82" t="s">
         <v>314</v>
       </c>
-      <c r="K81" t="s">
+      <c r="K82" t="s">
         <v>313</v>
       </c>
-      <c r="L81" t="s">
+      <c r="L82" t="s">
         <v>315</v>
       </c>
     </row>

</xml_diff>